<commit_message>
commit before refactor excel writeout
</commit_message>
<xml_diff>
--- a/vetting/regional/input_data/model_yaml_map.xlsx
+++ b/vetting/regional/input_data/model_yaml_map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\eu-climate-advisory-board-workflow\vetting\regional\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iiasahub.sharepoint.com/sites/eceprog/Shared Documents/Projects/EUAB/vetting/regional/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8AED98-01FB-4B63-B6B4-27C1D0C28000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{AB8AED98-01FB-4B63-B6B4-27C1D0C28000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C0AF565-B3D1-45F9-AED4-65FE32593239}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
   <si>
     <t>AIM/CGE 2.0</t>
   </si>
@@ -247,6 +247,18 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>R10_Europe</t>
+  </si>
+  <si>
+    <t>possibly only EU28?</t>
+  </si>
+  <si>
+    <t>native_iso_EU27</t>
   </si>
 </sst>
 </file>
@@ -564,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35:C43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +588,7 @@
     <col min="2" max="2" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -586,8 +598,11 @@
       <c r="C1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -598,7 +613,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -609,7 +624,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -620,15 +635,18 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
       <c r="C5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -639,15 +657,18 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
       <c r="C7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -655,7 +676,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -663,7 +684,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -674,7 +695,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -685,7 +706,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -696,7 +717,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -707,23 +728,29 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
       <c r="C15" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -734,7 +761,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -745,7 +772,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -756,7 +783,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -767,7 +794,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -778,7 +805,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -789,7 +816,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -800,7 +827,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -811,7 +838,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -822,23 +849,29 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="C25" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
+      <c r="B26" t="s">
+        <v>77</v>
+      </c>
       <c r="C26" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -846,31 +879,43 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
       <c r="C30" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -881,9 +926,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>77</v>
       </c>
       <c r="C32" t="s">
         <v>73</v>
@@ -893,6 +941,9 @@
       <c r="A33" t="s">
         <v>31</v>
       </c>
+      <c r="B33" t="s">
+        <v>77</v>
+      </c>
       <c r="C33" t="s">
         <v>73</v>
       </c>
@@ -901,6 +952,9 @@
       <c r="A34" t="s">
         <v>32</v>
       </c>
+      <c r="B34" t="s">
+        <v>77</v>
+      </c>
       <c r="C34" t="s">
         <v>73</v>
       </c>
@@ -912,6 +966,9 @@
       <c r="B35" t="s">
         <v>63</v>
       </c>
+      <c r="C35" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -920,6 +977,9 @@
       <c r="B36" t="s">
         <v>65</v>
       </c>
+      <c r="C36" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -928,6 +988,9 @@
       <c r="B37" t="s">
         <v>66</v>
       </c>
+      <c r="C37" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -936,6 +999,9 @@
       <c r="B38" t="s">
         <v>64</v>
       </c>
+      <c r="C38" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -944,6 +1010,9 @@
       <c r="B39" t="s">
         <v>64</v>
       </c>
+      <c r="C39" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -952,6 +1021,9 @@
       <c r="B40" t="s">
         <v>64</v>
       </c>
+      <c r="C40" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -960,6 +1032,9 @@
       <c r="B41" t="s">
         <v>65</v>
       </c>
+      <c r="C41" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -968,6 +1043,9 @@
       <c r="B42" t="s">
         <v>65</v>
       </c>
+      <c r="C42" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -975,6 +1053,9 @@
       </c>
       <c r="B43" t="s">
         <v>66</v>
+      </c>
+      <c r="C43" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>